<commit_message>
Update the document for table service
</commit_message>
<xml_diff>
--- a/routing_basic/resource/pictures/temp2.xlsx
+++ b/routing_basic/resource/pictures/temp2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xunliu/Desktop/git/telenav/open-source-spec/routing_basic/resource/pictures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45E7B64-16EE-FA48-A937-649CD83EC922}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81597959-A0C1-CF45-A54A-8601E2508271}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19620" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7899,6 +7899,714 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>101</xdr:col>
+      <xdr:colOff>77772</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>153785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>105</xdr:col>
+      <xdr:colOff>189175</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>92662</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="120" name="TextBox 119">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0B48630-CEEA-4C44-A375-A15C49A03183}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22611691" y="42990542"/>
+          <a:ext cx="1003835" cy="350769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>step1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>127</xdr:col>
+      <xdr:colOff>41388</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>117402</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>131</xdr:col>
+      <xdr:colOff>152791</xdr:colOff>
+      <xdr:row>211</xdr:row>
+      <xdr:rowOff>56279</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="121" name="TextBox 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C1F344-1DF0-C149-B4B4-D407DEBB7594}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28376118" y="43160105"/>
+          <a:ext cx="1003835" cy="350769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>step2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>154</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>158</xdr:col>
+      <xdr:colOff>111403</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>144823</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="124" name="TextBox 123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FC1BF5-2448-4D47-961C-6D1FF40B858B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34358649" y="43042703"/>
+          <a:ext cx="1003835" cy="350769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>step3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>104</xdr:col>
+      <xdr:colOff>201828</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>167501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>107</xdr:col>
+      <xdr:colOff>201827</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>150339</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="125" name="Right Arrow 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81191369-0236-A341-BBC1-E8D57A49243E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="23405071" y="31677231"/>
+          <a:ext cx="669324" cy="600676"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>105</xdr:col>
+      <xdr:colOff>92876</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>14428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>109</xdr:col>
+      <xdr:colOff>204278</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>159252</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="126" name="TextBox 125">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC49A785-644A-214A-949C-F2DB603E241C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23519227" y="32347942"/>
+          <a:ext cx="1003835" cy="350769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>step1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>119</xdr:col>
+      <xdr:colOff>148282</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>199766</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>122</xdr:col>
+      <xdr:colOff>148282</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>182604</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="Right Arrow 127">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FF267D4-2E78-EA48-B138-3508069B81D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="26698147" y="31709496"/>
+          <a:ext cx="669324" cy="600676"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>120</xdr:col>
+      <xdr:colOff>39330</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>46693</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>124</xdr:col>
+      <xdr:colOff>150733</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>191517</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="129" name="TextBox 128">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9E83982-FBBF-5A4A-B915-54C03252994B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26812303" y="32380207"/>
+          <a:ext cx="1003835" cy="350769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>step2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>135</xdr:col>
+      <xdr:colOff>43249</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>43247</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>138</xdr:col>
+      <xdr:colOff>43249</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>26085</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="131" name="Right Arrow 130">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0CDE88E-FD56-F643-AD0F-CB98B4EC1E37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="30162844" y="31758923"/>
+          <a:ext cx="669324" cy="600676"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>135</xdr:col>
+      <xdr:colOff>157405</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>96120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>140</xdr:col>
+      <xdr:colOff>45700</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>34998</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="132" name="TextBox 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E05B8AF7-D23A-3847-B14D-57573385038A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="30277000" y="32429634"/>
+          <a:ext cx="1003835" cy="350769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>step3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>181</xdr:col>
+      <xdr:colOff>24027</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>120134</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>184</xdr:col>
+      <xdr:colOff>24027</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>75512</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="150" name="Right Arrow 149">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBE23856-95EE-3343-9868-A4CA84CFB373}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="40406595" y="32041756"/>
+          <a:ext cx="669324" cy="573215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>181</xdr:col>
+      <xdr:colOff>138183</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>161584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>186</xdr:col>
+      <xdr:colOff>26478</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>84425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="151" name="TextBox 150">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAB14663-8653-0A49-B733-46320DA0A137}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="40520751" y="32701043"/>
+          <a:ext cx="1003835" cy="334733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>step4</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8184,8 +8892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="Z67:CF173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BL177" zoomScale="74" workbookViewId="0">
-      <selection activeCell="DE226" sqref="DE226"/>
+    <sheetView tabSelected="1" topLeftCell="AV182" zoomScale="74" workbookViewId="0">
+      <selection activeCell="DI224" sqref="DI224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>